<commit_message>
ci: update oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Cote d'Ivoire/civ_oncho_ia_202309_2_participant.xlsx
+++ b/ONCHO/Impact Assessments/Cote d'Ivoire/civ_oncho_ia_202309_2_participant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Cote d'Ivoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01FAA90-4A87-4DC1-8AB4-5A3F446F2893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E686E4-DD4D-4D9B-A1FB-C11498FFD1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>type</t>
   </si>
@@ -285,15 +285,9 @@
     <t>p_site_id</t>
   </si>
   <si>
-    <t>p_village_1ere_ligne</t>
-  </si>
-  <si>
     <t>4. Sélectionner le code du district</t>
   </si>
   <si>
-    <t>5. Sélectionner un village de 1ère ligne le plus proche</t>
-  </si>
-  <si>
     <t>6. Sélectionner le site d'enquête</t>
   </si>
   <si>
@@ -357,10 +351,10 @@
     <t>9.b. Code du participant</t>
   </si>
   <si>
-    <t>(Sept 2023) ONCHO Pre Stop - 2. Participants V3</t>
-  </si>
-  <si>
-    <t>civ_oncho_ia_202309_2_participant_v3</t>
+    <t>(Sept 2023) ONCHO Pre Stop - 2. Participants V3.1</t>
+  </si>
+  <si>
+    <t>civ_oncho_ia_202309_2_participant_v3_1</t>
   </si>
 </sst>
 </file>
@@ -836,13 +830,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -977,10 +971,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -993,132 +987,142 @@
       </c>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="31.5">
+    <row r="6" spans="1:13" s="7" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="8"/>
+      <c r="J6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:13" s="7" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="8"/>
       <c r="J7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" s="7" customFormat="1">
+    </row>
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="7" t="s">
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="31.5">
+      <c r="A9" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="31.5">
-      <c r="A10" s="24" t="s">
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1">
+      <c r="A10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="9" t="s">
+      <c r="B10" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="21" t="s">
-        <v>108</v>
-      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="19"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
-      <c r="M11" s="7" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1">
       <c r="A12" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="18"/>
@@ -1132,37 +1136,38 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1">
-      <c r="A13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="15" t="s">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1179,13 +1184,13 @@
     </row>
     <row r="15" spans="1:13" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1205,10 +1210,10 @@
         <v>20</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1228,10 +1233,10 @@
         <v>20</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1251,10 +1256,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1271,13 +1276,13 @@
     </row>
     <row r="19" spans="1:12" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1292,44 +1297,39 @@
       </c>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" spans="1:12" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" s="10"/>
-    </row>
-    <row r="21" spans="1:12" s="7" customFormat="1" ht="31.5">
+    <row r="20" spans="1:12" s="7" customFormat="1" ht="31.5">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" s="7" customFormat="1">
       <c r="A21" s="9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>103</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="8"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="10"/>
       <c r="K21" s="9"/>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="22" spans="1:12" s="7" customFormat="1">
       <c r="A22" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1354,12 +1354,8 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" s="7" customFormat="1">
-      <c r="A23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>69</v>
-      </c>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="9"/>
@@ -1372,18 +1368,9 @@
       <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12" s="7" customFormat="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1">
       <c r="B25" s="8"/>
@@ -1391,14 +1378,9 @@
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" s="7" customFormat="1">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1826,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1853,10 +1835,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>

</xml_diff>